<commit_message>
Added icon to ENOVAEmblems
New RU localization files for CustomLocalization
</commit_message>
<xml_diff>
--- a/CustomLocalization/Localization/RogueTech/RU/AbilityRealizer/LocalizationDef.xlsx
+++ b/CustomLocalization/Localization/RogueTech/RU/AbilityRealizer/LocalizationDef.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="259">
   <si>
     <t>ID</t>
   </si>
@@ -40,7 +40,7 @@
     <t>PASSIVE: Reduces Heat generation by 10%.</t>
   </si>
   <si>
-    <t>PASSIVE: генерация тепла снижена на 10%</t>
+    <t>ПАССИВНО: генерация тепла снижена на 10%</t>
   </si>
   <si>
     <t>TraitClanner.StatusEffect_Cockpit_Skill_Gunnery.EffectData0.Name</t>
@@ -85,7 +85,7 @@
     <t>Hand Melee Damage</t>
   </si>
   <si>
-    <t>Урон рукопашной</t>
+    <t>Урон в рукопашной</t>
   </si>
   <si>
     <t>TraitClanner.StatusEffect-ClannerDebuffDFAStab.EffectData5.Name</t>
@@ -187,7 +187,7 @@
     <t>-10% Heat Generation</t>
   </si>
   <si>
-    <t>-10% генер. тепла</t>
+    <t>-10% генерация тепла</t>
   </si>
   <si>
     <t>TraitComstar.Description.Name</t>
@@ -593,6 +593,204 @@
   </si>
   <si>
     <t>TraitClanner_HH.StatusEffect-ClannerDebuffMeleeStab.EffectData5.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner.DNI_Damage_Charge.EffectData12.Details</t>
+  </si>
+  <si>
+    <t>Damage Modifier</t>
+  </si>
+  <si>
+    <t>Модификатор урона</t>
+  </si>
+  <si>
+    <t>TraitClanner.DNI_Damage_Charge.EffectData12.Name</t>
+  </si>
+  <si>
+    <t>Melee Weapon Damage Mod</t>
+  </si>
+  <si>
+    <t>Рукоп. оружие урон</t>
+  </si>
+  <si>
+    <t>TraitClanner.DNI_Damage_Charge.EffectData7.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner.DNI_Damage_Charge.EffectData7.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner.DNI_Damage_DFA.EffectData13.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner.DNI_Damage_DFA.EffectData13.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner.DNI_Damage_DFA.EffectData8.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner.DNI_Damage_DFA.EffectData8.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner.DNI_Damage_Kick.EffectData11.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner.DNI_Damage_Kick.EffectData11.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner.DNI_Damage_Kick.EffectData6.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner.DNI_Damage_Kick.EffectData6.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner.DNI_Damage_Punch.EffectData10.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner.DNI_Damage_Punch.EffectData10.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner.DNI_Damage_Punch.EffectData5.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner.DNI_Damage_Punch.EffectData5.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner.DNI_Damage_Weapon.EffectData4.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner.DNI_Damage_Weapon.EffectData4.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner.DNI_Damage_Weapon.EffectData9.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner.DNI_Damage_Weapon.EffectData9.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner.FCS_MeleeAccuracy.EffectData14.Details</t>
+  </si>
+  <si>
+    <t>MeleeWeapon Accuracy Modifier</t>
+  </si>
+  <si>
+    <t>Рукоп. оруж. точность</t>
+  </si>
+  <si>
+    <t>TraitClanner.FCS_MeleeAccuracy.EffectData14.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner.FCS_MeleeAccuracy.EffectData15.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner.FCS_MeleeAccuracy.EffectData15.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner.FCS_MeleeAccuracy.EffectData16.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner.FCS_MeleeAccuracy.EffectData16.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner.FCS_MeleeAccuracy.EffectData17.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner.FCS_MeleeAccuracy.EffectData17.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner.FCS_MeleeAccuracy.EffectData18.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner.FCS_MeleeAccuracy.EffectData18.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.DNI_Damage_Charge.EffectData10.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.DNI_Damage_Charge.EffectData10.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.DNI_Damage_Charge.EffectData5.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.DNI_Damage_Charge.EffectData5.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.DNI_Damage_DFA.EffectData11.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.DNI_Damage_DFA.EffectData11.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.DNI_Damage_DFA.EffectData6.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.DNI_Damage_DFA.EffectData6.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.DNI_Damage_Kick.EffectData4.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.DNI_Damage_Kick.EffectData4.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.DNI_Damage_Kick.EffectData9.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.DNI_Damage_Kick.EffectData9.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.DNI_Damage_Punch.EffectData3.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.DNI_Damage_Punch.EffectData3.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.DNI_Damage_Punch.EffectData8.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.DNI_Damage_Punch.EffectData8.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.DNI_Damage_Weapon.EffectData2.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.DNI_Damage_Weapon.EffectData2.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.DNI_Damage_Weapon.EffectData7.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.DNI_Damage_Weapon.EffectData7.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.FCS_MeleeAccuracy.EffectData12.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.FCS_MeleeAccuracy.EffectData12.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.FCS_MeleeAccuracy.EffectData13.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.FCS_MeleeAccuracy.EffectData13.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.FCS_MeleeAccuracy.EffectData14.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.FCS_MeleeAccuracy.EffectData14.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.FCS_MeleeAccuracy.EffectData15.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.FCS_MeleeAccuracy.EffectData15.Name</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.FCS_MeleeAccuracy.EffectData16.Details</t>
+  </si>
+  <si>
+    <t>TraitClanner_HH.FCS_MeleeAccuracy.EffectData16.Name</t>
   </si>
 </sst>
 </file>
@@ -626,13 +824,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" quotePrefix="1" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -640,9 +843,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -680,7 +883,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -750,7 +953,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -924,1570 +1127,2412 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D136"/>
+  <dimension ref="A1:D196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="B190" sqref="B190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="1" width="75.7109375" customWidth="1"/>
+    <col min="1" max="1" bestFit="1" width="75.7109375" customWidth="1" style="2"/>
+    <col min="2" max="3" width="53.140625" customWidth="1" style="2"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1" style="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C52" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C53" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="C54" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C55" s="0" t="s">
+      <c r="C55" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="C56" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C57" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="B58" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="C58" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B59" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C59" s="0" t="s">
+      <c r="C59" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B60" s="0" t="s">
+      <c r="B60" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C60" s="0" t="s">
+      <c r="C60" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="B61" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="C61" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="B62" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="C62" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B63" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C63" s="0" t="s">
+      <c r="C63" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B64" s="0" t="s">
+      <c r="B64" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C64" s="0" t="s">
+      <c r="C64" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C65" s="0" t="s">
+      <c r="C65" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B66" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="0" t="s">
+      <c r="C66" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="s">
+      <c r="A67" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B67" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C67" s="0" t="s">
+      <c r="C67" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="B68" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C68" s="0" t="s">
+      <c r="C68" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="B69" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C69" s="0" t="s">
+      <c r="C69" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B70" s="0" t="s">
+      <c r="B70" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C70" s="0" t="s">
+      <c r="C70" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B71" s="0" t="s">
+      <c r="B71" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C71" s="0" t="s">
+      <c r="C71" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B72" s="0" t="s">
+      <c r="B72" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C72" s="0" t="s">
+      <c r="C72" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B73" s="0" t="s">
+      <c r="B73" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C73" s="0" t="s">
+      <c r="C73" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="1" t="s">
+      <c r="A74" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B74" s="0" t="s">
+      <c r="B74" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C74" s="0" t="s">
+      <c r="C74" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B75" s="0" t="s">
+      <c r="B75" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C75" s="0" t="s">
+      <c r="C75" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B76" s="0" t="s">
+      <c r="B76" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C76" s="0" t="s">
+      <c r="C76" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B77" s="0" t="s">
+      <c r="B77" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C77" s="0" t="s">
+      <c r="C77" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B78" s="0" t="s">
+      <c r="B78" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C78" s="0" t="s">
+      <c r="C78" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B79" s="0" t="s">
+      <c r="B79" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C79" s="0" t="s">
+      <c r="C79" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="0" t="s">
+      <c r="A80" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B80" s="0" t="s">
+      <c r="B80" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C80" s="0" t="s">
+      <c r="C80" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="1" t="s">
+      <c r="A81" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B81" s="0" t="s">
+      <c r="B81" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C81" s="0" t="s">
+      <c r="C81" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B82" s="0" t="s">
+      <c r="B82" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C82" s="0" t="s">
+      <c r="C82" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="1" t="s">
+      <c r="A83" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B83" s="0" t="s">
+      <c r="B83" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C83" s="0" t="s">
+      <c r="C83" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="1" t="s">
+      <c r="A84" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B84" s="0" t="s">
+      <c r="B84" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C84" s="0" t="s">
+      <c r="C84" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="0" t="s">
+      <c r="A85" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B85" s="0" t="s">
+      <c r="B85" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C85" s="0" t="s">
+      <c r="C85" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B86" s="0" t="s">
+      <c r="B86" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C86" s="0" t="s">
+      <c r="C86" s="2" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="1" t="s">
+      <c r="A87" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B87" s="0" t="s">
+      <c r="B87" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C87" s="0" t="s">
+      <c r="C87" s="2" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="1" t="s">
+      <c r="A88" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B88" s="0" t="s">
+      <c r="B88" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C88" s="0" t="s">
+      <c r="C88" s="2" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="1" t="s">
+      <c r="A89" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B89" s="0" t="s">
+      <c r="B89" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C89" s="0" t="s">
+      <c r="C89" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="0" t="s">
+      <c r="A90" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B90" s="0" t="s">
+      <c r="B90" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C90" s="0" t="s">
+      <c r="C90" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="1" t="s">
+      <c r="A91" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B91" s="0" t="s">
+      <c r="B91" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C91" s="0" t="s">
+      <c r="C91" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="1" t="s">
+      <c r="A92" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B92" s="0" t="s">
+      <c r="B92" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C92" s="0" t="s">
+      <c r="C92" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="1" t="s">
+      <c r="A93" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B93" s="0" t="s">
+      <c r="B93" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C93" s="0" t="s">
+      <c r="C93" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="1" t="s">
+      <c r="A94" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B94" s="0" t="s">
+      <c r="B94" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C94" s="0" t="s">
+      <c r="C94" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="1" t="s">
+      <c r="A95" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B95" s="0" t="s">
+      <c r="B95" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C95" s="0" t="s">
+      <c r="C95" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="1" t="s">
+      <c r="A96" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B96" s="0" t="s">
+      <c r="B96" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C96" s="0" t="s">
+      <c r="C96" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="1" t="s">
+      <c r="A97" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B97" s="0" t="s">
+      <c r="B97" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C97" s="0" t="s">
+      <c r="C97" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="1" t="s">
+      <c r="A98" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B98" s="0" t="s">
+      <c r="B98" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C98" s="0" t="s">
+      <c r="C98" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="1" t="s">
+      <c r="A99" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B99" s="0" t="s">
+      <c r="B99" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C99" s="0" t="s">
+      <c r="C99" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="1" t="s">
+      <c r="A100" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B100" s="0" t="s">
+      <c r="B100" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C100" s="0" t="s">
+      <c r="C100" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="0" t="s">
+      <c r="A101" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B101" s="0" t="s">
+      <c r="B101" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C101" s="0" t="s">
+      <c r="C101" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="1" t="s">
+      <c r="A102" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B102" s="0" t="s">
+      <c r="B102" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C102" s="0" t="s">
+      <c r="C102" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="1" t="s">
+      <c r="A103" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B103" s="0" t="s">
+      <c r="B103" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C103" s="0" t="s">
+      <c r="C103" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="1" t="s">
+      <c r="A104" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B104" s="0" t="s">
+      <c r="B104" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C104" s="0" t="s">
+      <c r="C104" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="1" t="s">
+      <c r="A105" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B105" s="0" t="s">
+      <c r="B105" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C105" s="0" t="s">
+      <c r="C105" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="1" t="s">
+      <c r="A106" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B106" s="0" t="s">
+      <c r="B106" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C106" s="0" t="s">
+      <c r="C106" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="1" t="s">
+      <c r="A107" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B107" s="0" t="s">
+      <c r="B107" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C107" s="0" t="s">
+      <c r="C107" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="1" t="s">
+      <c r="A108" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B108" s="0" t="s">
+      <c r="B108" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C108" s="0" t="s">
+      <c r="C108" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="1" t="s">
+      <c r="A109" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B109" s="0" t="s">
+      <c r="B109" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C109" s="0" t="s">
+      <c r="C109" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="1" t="s">
+      <c r="A110" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B110" s="0" t="s">
+      <c r="B110" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C110" s="0" t="s">
+      <c r="C110" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="1" t="s">
+      <c r="A111" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B111" s="0" t="s">
+      <c r="B111" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C111" s="0" t="s">
+      <c r="C111" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="0" t="s">
+      <c r="A112" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B112" s="0" t="s">
+      <c r="B112" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C112" s="0" t="s">
+      <c r="C112" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="1" t="s">
+      <c r="A113" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B113" s="0" t="s">
+      <c r="B113" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C113" s="0" t="s">
+      <c r="C113" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="1" t="s">
+      <c r="A114" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B114" s="0" t="s">
+      <c r="B114" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C114" s="0" t="s">
+      <c r="C114" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="1" t="s">
+      <c r="A115" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B115" s="0" t="s">
+      <c r="B115" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C115" s="0" t="s">
+      <c r="C115" s="2" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="1" t="s">
+      <c r="A116" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="B116" s="0" t="s">
+      <c r="B116" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C116" s="0" t="s">
+      <c r="C116" s="2" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="0" t="s">
+      <c r="A117" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B117" s="0" t="s">
+      <c r="B117" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C117" s="0" t="s">
+      <c r="C117" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="0" t="s">
+      <c r="A118" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B118" s="0" t="s">
+      <c r="B118" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C118" s="0" t="s">
+      <c r="C118" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D118" s="0" t="s">
+      <c r="D118" s="2" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="0" t="s">
+      <c r="A119" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B119" s="0" t="s">
+      <c r="B119" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C119" s="0" t="s">
+      <c r="C119" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D119" s="0" t="s">
+      <c r="D119" s="2" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="0" t="s">
+      <c r="A120" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B120" s="0" t="s">
+      <c r="B120" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C120" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="D120" s="0" t="s">
+      <c r="C120" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D120" s="2" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="0" t="s">
+      <c r="A121" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B121" s="0" t="s">
+      <c r="B121" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C121" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D121" s="0" t="s">
+      <c r="C121" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D121" s="2" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="0" t="s">
+      <c r="A122" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B122" s="0" t="s">
+      <c r="B122" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C122" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D122" s="0" t="s">
+      <c r="C122" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D122" s="2" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="0" t="s">
+      <c r="A123" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B123" s="0" t="s">
+      <c r="B123" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C123" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D123" s="0" t="s">
+      <c r="C123" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D123" s="2" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="0" t="s">
+      <c r="A124" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B124" s="0" t="s">
+      <c r="B124" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C124" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D124" s="0" t="s">
+      <c r="C124" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D124" s="2" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="0" t="s">
+      <c r="A125" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B125" s="0" t="s">
+      <c r="B125" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C125" s="0" t="s">
+      <c r="C125" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B127" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D125" s="0" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="B126" s="0" t="s">
+      <c r="C127" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B128" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C126" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D126" s="0" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="B127" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C127" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="D127" s="0" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="B128" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C128" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D128" s="0" t="s">
+      <c r="C128" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D128" s="2" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="0" t="s">
+      <c r="A129" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B129" s="0" t="s">
+      <c r="B129" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C129" s="0" t="s">
+      <c r="C129" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B133" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D129" s="0" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="B130" s="0" t="s">
+      <c r="C133" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B134" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C130" s="0" t="s">
+      <c r="C134" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B136" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D130" s="0" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="B131" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C131" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="D131" s="0" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="B132" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C132" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D132" s="0" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="B133" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C133" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="D133" s="0" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="B134" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C134" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D134" s="0" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="B135" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C135" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="D135" s="0" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="B136" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C136" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D136" s="0" t="s">
+      <c r="C136" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C137" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C138" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C139" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C140" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C141" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C142" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B143" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C143" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C144" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C145" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C146" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C147" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C148" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B149" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C149" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B150" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C150" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B151" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C151" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C152" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B153" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C153" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B154" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C154" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B155" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C155" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B156" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C156" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C157" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B158" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C158" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B159" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C159" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B160" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C160" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B161" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C161" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B162" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C162" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C163" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B164" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C164" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D164" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B165" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C165" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D165" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B166" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C166" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B167" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C167" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B168" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C168" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B169" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C169" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D169" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B170" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C170" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B171" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C171" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B172" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C172" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D172" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B173" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C173" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B174" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C174" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D174" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B175" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C175" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D175" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B176" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C176" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D176" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B177" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C177" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D177" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B178" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C178" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D178" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B179" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C179" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D179" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B180" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C180" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B181" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C181" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D181" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B182" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C182" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D182" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B183" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C183" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D183" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B184" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C184" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D184" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B185" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C185" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D185" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B186" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C186" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D186" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B187" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C187" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D187" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B188" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C188" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D188" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B189" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C189" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D189" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B190" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C190" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D190" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B191" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C191" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D191" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B192" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C192" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D192" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B193" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C193" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D193" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B194" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C194" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D194" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B195" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C195" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D195" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B196" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C196" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D196" s="2" t="s">
         <v>173</v>
       </c>
     </row>

</xml_diff>